<commit_message>
feature(): Modelos de mensagens import
</commit_message>
<xml_diff>
--- a/public/modelos/Envia_modelos_mensagens.xlsx
+++ b/public/modelos/Envia_modelos_mensagens.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\projects\project-hawk\hotsite\planilhas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\nodejs\envia-backend\public\modelos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7564429D-890B-4C47-AFC5-12B576041CFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFF886FC-37D1-4FE3-A204-CFBAF367D72A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,9 +32,6 @@
   </si>
   <si>
     <t>Saudação da Mensagem</t>
-  </si>
-  <si>
-    <t>ex.: Modelo de Parabenização para Aniversários</t>
   </si>
   <si>
     <r>
@@ -85,9 +82,6 @@
     </r>
   </si>
   <si>
-    <t>ex.: É Ótimo tê-lo conosco! Feliz aniversário!</t>
-  </si>
-  <si>
     <t>Modelo de Parabenização</t>
   </si>
   <si>
@@ -95,6 +89,12 @@
   </si>
   <si>
     <t>É ótimo tê-lo conosco! Feliz aniversário!</t>
+  </si>
+  <si>
+    <t>ex.: Feliz aniversário [NOME]!</t>
+  </si>
+  <si>
+    <t>ex.: É Ótimo tê-lo conosco! Feliz aniversário [NOME]!</t>
   </si>
 </sst>
 </file>
@@ -535,7 +535,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -563,24 +563,24 @@
     </row>
     <row r="3" spans="1:3" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>5</v>
-      </c>
       <c r="C3" s="4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>